<commit_message>
bash script for grid search
</commit_message>
<xml_diff>
--- a/HINGCN-GS/pytorch-graphsage-master/experiment/results.xlsx
+++ b/HINGCN-GS/pytorch-graphsage-master/experiment/results.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBAACA20-0F09-4038-88C7-2675A9A273D2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF397F72-BADF-41CA-B623-A1BCD974B705}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -13,17 +13,23 @@
     <sheet name="freebase" sheetId="4" r:id="rId3"/>
     <sheet name="scripts" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="42">
   <si>
     <t>Validation</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -177,6 +183,10 @@
   </si>
   <si>
     <t>baseline</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>grid search</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1526,11 +1536,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{615B164C-2941-49E7-A89D-E66BEB08CEB9}">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
+      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1730,6 +1740,12 @@
       </c>
     </row>
     <row r="7" spans="1:12">
+      <c r="A7" s="5">
+        <v>62.1</v>
+      </c>
+      <c r="B7" s="5">
+        <v>64.5</v>
+      </c>
       <c r="C7" s="5">
         <v>3.0000000000000001E-3</v>
       </c>
@@ -1756,6 +1772,11 @@
       </c>
       <c r="K7" s="5" t="b">
         <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="3" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1770,7 +1791,7 @@
   <dimension ref="A3:Z3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="A3" sqref="A3:Z3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>

</xml_diff>

<commit_message>
added logistic regreesion for node2vec
</commit_message>
<xml_diff>
--- a/HINGCN-GS/pytorch-graphsage-master/experiment/results.xlsx
+++ b/HINGCN-GS/pytorch-graphsage-master/experiment/results.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF397F72-BADF-41CA-B623-A1BCD974B705}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0457EEE6-9BC4-4C52-9D60-920ECCA342FA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="49">
   <si>
     <t>Validation</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -187,6 +187,33 @@
   </si>
   <si>
     <t>grid search</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>attention</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Early stopping</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dropout</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Logistic </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Regreesion</t>
+  </si>
+  <si>
+    <t>ON</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Node2Vec</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -258,7 +285,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -283,6 +310,12 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1365,10 +1398,10 @@
       <c r="C44" s="1">
         <v>0.01</v>
       </c>
-      <c r="D44" s="7" t="s">
+      <c r="D44" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="E44" s="7"/>
+      <c r="E44" s="10"/>
       <c r="H44" s="1" t="s">
         <v>30</v>
       </c>
@@ -1392,10 +1425,10 @@
       <c r="C45" s="4">
         <v>0.01</v>
       </c>
-      <c r="D45" s="7" t="s">
+      <c r="D45" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="E45" s="7"/>
+      <c r="E45" s="10"/>
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
       <c r="H45" s="4" t="s">
@@ -1421,10 +1454,10 @@
       <c r="C46" s="5">
         <v>0.01</v>
       </c>
-      <c r="D46" s="7" t="s">
+      <c r="D46" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="E46" s="7"/>
+      <c r="E46" s="10"/>
       <c r="H46" s="1" t="s">
         <v>33</v>
       </c>
@@ -1448,10 +1481,10 @@
       <c r="C47" s="5">
         <v>0.01</v>
       </c>
-      <c r="D47" s="7" t="s">
+      <c r="D47" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="E47" s="7"/>
+      <c r="E47" s="10"/>
       <c r="H47" s="1" t="s">
         <v>34</v>
       </c>
@@ -1475,10 +1508,10 @@
       <c r="C48" s="5">
         <v>0.01</v>
       </c>
-      <c r="D48" s="7" t="s">
+      <c r="D48" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="E48" s="7"/>
+      <c r="E48" s="10"/>
       <c r="F48" s="5"/>
       <c r="G48" s="5"/>
       <c r="H48" s="5" t="s">
@@ -1500,10 +1533,10 @@
       <c r="C49" s="5">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="D49" s="7" t="s">
+      <c r="D49" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="E49" s="7"/>
+      <c r="E49" s="10"/>
       <c r="F49" s="5"/>
       <c r="G49" s="5"/>
       <c r="H49" s="5" t="s">
@@ -1536,24 +1569,24 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{615B164C-2941-49E7-A89D-E66BEB08CEB9}">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="3" width="9" style="5"/>
-    <col min="4" max="4" width="14.5" style="5" customWidth="1"/>
-    <col min="5" max="5" width="9.75" style="5" customWidth="1"/>
-    <col min="6" max="6" width="11.375" style="5" customWidth="1"/>
+    <col min="4" max="4" width="14.5" style="5" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="9.375" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.375" style="5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.25" style="5" customWidth="1"/>
     <col min="8" max="8" width="16.75" style="5" customWidth="1"/>
     <col min="9" max="9" width="14.75" style="5" customWidth="1"/>
-    <col min="10" max="10" width="13.125" style="5" customWidth="1"/>
-    <col min="11" max="11" width="13.375" style="5" customWidth="1"/>
+    <col min="10" max="10" width="13.125" style="5" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="13.375" style="5" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="16.625" style="5" customWidth="1"/>
     <col min="13" max="16384" width="9" style="5"/>
   </cols>
@@ -1572,7 +1605,7 @@
         <v>4</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>6</v>
@@ -1777,6 +1810,521 @@
     <row r="9" spans="1:12">
       <c r="A9" s="3" t="s">
         <v>41</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="5">
+        <v>49</v>
+      </c>
+      <c r="B10" s="5">
+        <v>47.9</v>
+      </c>
+      <c r="C10" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="E10" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="F10" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="5">
+        <v>50.1</v>
+      </c>
+      <c r="B11" s="5">
+        <v>51.5</v>
+      </c>
+      <c r="C11" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="E11" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="F11" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="5">
+        <v>44.5</v>
+      </c>
+      <c r="B12" s="5">
+        <v>44.6</v>
+      </c>
+      <c r="C12" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="E12" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="F12" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="5">
+        <v>48.1</v>
+      </c>
+      <c r="B13" s="5">
+        <v>50.1</v>
+      </c>
+      <c r="C13" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="E13" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="F13" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="5">
+        <v>52.6</v>
+      </c>
+      <c r="B14" s="5">
+        <v>50.1</v>
+      </c>
+      <c r="C14" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="E14" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="F14" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="5">
+        <v>49</v>
+      </c>
+      <c r="B15" s="5">
+        <v>50.1</v>
+      </c>
+      <c r="C15" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="E15" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="F15" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="5">
+        <v>57.9</v>
+      </c>
+      <c r="B16" s="5">
+        <v>60.2</v>
+      </c>
+      <c r="C16" s="7">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="E16" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="F16" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="I16" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="5">
+        <v>61.2</v>
+      </c>
+      <c r="B17" s="5">
+        <v>63.4</v>
+      </c>
+      <c r="C17" s="7">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="E17" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="F17" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="5">
+        <v>62.4</v>
+      </c>
+      <c r="B18" s="5">
+        <v>63.4</v>
+      </c>
+      <c r="C18" s="7">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="E18" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="F18" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="I18" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="5">
+        <v>49.2</v>
+      </c>
+      <c r="B19" s="5">
+        <v>51.4</v>
+      </c>
+      <c r="C19" s="7">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="E19" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="F19" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H19" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="I19" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" s="5">
+        <v>44.7</v>
+      </c>
+      <c r="B20" s="5">
+        <v>44.8</v>
+      </c>
+      <c r="C20" s="7">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="E20" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="F20" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="I20" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="5">
+        <v>51.8</v>
+      </c>
+      <c r="B21" s="5">
+        <v>52.8</v>
+      </c>
+      <c r="C21" s="7">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="E21" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="F21" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H21" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="I21" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" s="5">
+        <v>45.7</v>
+      </c>
+      <c r="B22" s="5">
+        <v>46.9</v>
+      </c>
+      <c r="C22" s="5">
+        <v>1E-3</v>
+      </c>
+      <c r="E22" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="F22" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H22" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="I22" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" s="9">
+        <v>59.341000000000001</v>
+      </c>
+      <c r="B23" s="9">
+        <v>63.09</v>
+      </c>
+      <c r="C23" s="7">
+        <v>1E-3</v>
+      </c>
+      <c r="E23" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="F23" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H23" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="I23" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" s="3">
+        <v>61.203000000000003</v>
+      </c>
+      <c r="B24" s="3">
+        <v>64.807000000000002</v>
+      </c>
+      <c r="C24" s="7">
+        <v>1E-3</v>
+      </c>
+      <c r="E24" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="F24" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H24" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="I24" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" s="9">
+        <v>44.595999999999997</v>
+      </c>
+      <c r="B25" s="9">
+        <v>44.920999999999999</v>
+      </c>
+      <c r="C25" s="7">
+        <v>1E-3</v>
+      </c>
+      <c r="E25" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="F25" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H25" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="I25" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" s="9">
+        <v>44.667000000000002</v>
+      </c>
+      <c r="B26" s="9">
+        <v>44.777999999999999</v>
+      </c>
+      <c r="C26" s="7">
+        <v>1E-3</v>
+      </c>
+      <c r="E26" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="F26" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H26" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="I26" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" s="9">
+        <v>53.329000000000001</v>
+      </c>
+      <c r="B27" s="9">
+        <v>55.508000000000003</v>
+      </c>
+      <c r="C27" s="7">
+        <v>1E-3</v>
+      </c>
+      <c r="E27" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="F27" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H27" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="I27" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="C30" s="9">
+        <v>1E-3</v>
+      </c>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9">
+        <v>0</v>
+      </c>
+      <c r="F30" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="G30" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="H30" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="I30" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32" s="5">
+        <v>68.146000000000001</v>
+      </c>
+      <c r="B32" s="5">
+        <v>73.103999999999999</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1790,41 +2338,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA8F9CC4-0108-45EF-9527-DD6242459EC5}">
   <dimension ref="A3:Z3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3:Z3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="3" spans="1:26">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
-      <c r="O3" s="7"/>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="7"/>
-      <c r="R3" s="7"/>
-      <c r="S3" s="7"/>
-      <c r="T3" s="7"/>
-      <c r="U3" s="7"/>
-      <c r="V3" s="7"/>
-      <c r="W3" s="7"/>
-      <c r="X3" s="7"/>
-      <c r="Y3" s="7"/>
-      <c r="Z3" s="7"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="10"/>
+      <c r="R3" s="10"/>
+      <c r="S3" s="10"/>
+      <c r="T3" s="10"/>
+      <c r="U3" s="10"/>
+      <c r="V3" s="10"/>
+      <c r="W3" s="10"/>
+      <c r="X3" s="10"/>
+      <c r="Y3" s="10"/>
+      <c r="Z3" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
attention head; multi-layer GCN;
</commit_message>
<xml_diff>
--- a/HINGCN-GS/pytorch-graphsage-master/experiment/results.xlsx
+++ b/HINGCN-GS/pytorch-graphsage-master/experiment/results.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42CFD884-E630-4E7E-BCF5-76DC299FEA71}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4006F16A-C4A9-411A-A237-65D02E75011E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,6 @@
     <sheet name="scripts" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="61">
   <si>
     <t>Validation</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -251,6 +250,18 @@
   </si>
   <si>
     <t>overfitting</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>16-&gt;32-&gt;16-&gt;3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>concat edge</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>concat node</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -335,7 +346,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -371,6 +382,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -671,9 +685,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80816BB4-F10A-443F-9268-185E0F570021}">
   <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1474,10 +1488,10 @@
       <c r="C44" s="1">
         <v>0.01</v>
       </c>
-      <c r="D44" s="13" t="s">
+      <c r="D44" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="E44" s="13"/>
+      <c r="E44" s="14"/>
       <c r="H44" s="1" t="s">
         <v>30</v>
       </c>
@@ -1501,10 +1515,10 @@
       <c r="C45" s="4">
         <v>0.01</v>
       </c>
-      <c r="D45" s="13" t="s">
+      <c r="D45" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="E45" s="13"/>
+      <c r="E45" s="14"/>
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
       <c r="H45" s="4" t="s">
@@ -1530,10 +1544,10 @@
       <c r="C46" s="5">
         <v>0.01</v>
       </c>
-      <c r="D46" s="13" t="s">
+      <c r="D46" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="E46" s="13"/>
+      <c r="E46" s="14"/>
       <c r="H46" s="1" t="s">
         <v>33</v>
       </c>
@@ -1557,10 +1571,10 @@
       <c r="C47" s="5">
         <v>0.01</v>
       </c>
-      <c r="D47" s="13" t="s">
+      <c r="D47" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="E47" s="13"/>
+      <c r="E47" s="14"/>
       <c r="H47" s="1" t="s">
         <v>34</v>
       </c>
@@ -1584,10 +1598,10 @@
       <c r="C48" s="5">
         <v>0.01</v>
       </c>
-      <c r="D48" s="13" t="s">
+      <c r="D48" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="E48" s="13"/>
+      <c r="E48" s="14"/>
       <c r="F48" s="5"/>
       <c r="G48" s="5"/>
       <c r="H48" s="5" t="s">
@@ -1609,10 +1623,10 @@
       <c r="C49" s="5">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="D49" s="13" t="s">
+      <c r="D49" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="E49" s="13"/>
+      <c r="E49" s="14"/>
       <c r="F49" s="5"/>
       <c r="G49" s="5"/>
       <c r="H49" s="5" t="s">
@@ -1645,11 +1659,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{615B164C-2941-49E7-A89D-E66BEB08CEB9}">
-  <dimension ref="A1:M43"/>
+  <dimension ref="A1:M50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E45" sqref="E45"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E49" sqref="E49:M49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2668,6 +2682,12 @@
       </c>
     </row>
     <row r="43" spans="1:13">
+      <c r="A43" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B43" s="12" t="s">
+        <v>56</v>
+      </c>
       <c r="C43" s="10">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -2691,6 +2711,218 @@
       <c r="K43" s="10"/>
       <c r="L43" s="10" t="s">
         <v>55</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13">
+      <c r="A44" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B44" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="C44" s="10">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D44" s="10"/>
+      <c r="E44" s="10">
+        <v>0</v>
+      </c>
+      <c r="F44" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="G44" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H44" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="I44" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J44" s="10"/>
+      <c r="K44" s="10"/>
+      <c r="L44" s="10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13">
+      <c r="A45" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B45" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="C45" s="10">
+        <v>1E-3</v>
+      </c>
+      <c r="D45" s="10"/>
+      <c r="E45" s="10">
+        <v>0</v>
+      </c>
+      <c r="F45" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="G45" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H45" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="I45" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J45" s="10"/>
+      <c r="K45" s="10"/>
+      <c r="L45" s="10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13">
+      <c r="C46" s="10">
+        <v>1E-3</v>
+      </c>
+      <c r="D46" s="10"/>
+      <c r="E46" s="10">
+        <v>0</v>
+      </c>
+      <c r="F46" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="G46" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H46" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="I46" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J46" s="10"/>
+      <c r="K46" s="10"/>
+      <c r="L46" s="10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13">
+      <c r="C47" s="10">
+        <v>1E-3</v>
+      </c>
+      <c r="D47" s="10"/>
+      <c r="E47" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="F47" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="G47" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H47" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="I47" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J47" s="10"/>
+      <c r="K47" s="10"/>
+      <c r="L47" s="10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13">
+      <c r="A48" s="5">
+        <v>65</v>
+      </c>
+      <c r="B48" s="5">
+        <v>66.8</v>
+      </c>
+      <c r="C48" s="13">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D48" s="13"/>
+      <c r="E48" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="F48" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="G48" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="H48" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="I48" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J48" s="13"/>
+      <c r="K48" s="13"/>
+      <c r="L48" s="13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" ht="15">
+      <c r="A49" s="8">
+        <v>64.924999999999997</v>
+      </c>
+      <c r="B49" s="8">
+        <v>68.956000000000003</v>
+      </c>
+      <c r="C49" s="13">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="F49" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="G49" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="H49" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="I49" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J49" s="13"/>
+      <c r="K49" s="13"/>
+      <c r="L49" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="M49" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13">
+      <c r="C50" s="13">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D50" s="13"/>
+      <c r="E50" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="F50" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="G50" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="H50" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="I50" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J50" s="13"/>
+      <c r="K50" s="13"/>
+      <c r="L50" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="M50" s="13" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -2711,34 +2943,34 @@
   <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="3" spans="1:26">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="13"/>
-      <c r="N3" s="13"/>
-      <c r="O3" s="13"/>
-      <c r="P3" s="13"/>
-      <c r="Q3" s="13"/>
-      <c r="R3" s="13"/>
-      <c r="S3" s="13"/>
-      <c r="T3" s="13"/>
-      <c r="U3" s="13"/>
-      <c r="V3" s="13"/>
-      <c r="W3" s="13"/>
-      <c r="X3" s="13"/>
-      <c r="Y3" s="13"/>
-      <c r="Z3" s="13"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="14"/>
+      <c r="P3" s="14"/>
+      <c r="Q3" s="14"/>
+      <c r="R3" s="14"/>
+      <c r="S3" s="14"/>
+      <c r="T3" s="14"/>
+      <c r="U3" s="14"/>
+      <c r="V3" s="14"/>
+      <c r="W3" s="14"/>
+      <c r="X3" s="14"/>
+      <c r="Y3" s="14"/>
+      <c r="Z3" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
test of GCN on datasets
</commit_message>
<xml_diff>
--- a/HINGCN-GS/pytorch-graphsage-master/experiment/results.xlsx
+++ b/HINGCN-GS/pytorch-graphsage-master/experiment/results.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4006F16A-C4A9-411A-A237-65D02E75011E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42F908F4-BE06-484E-966E-91C3918558F7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="71">
   <si>
     <t>Validation</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -262,6 +262,46 @@
   </si>
   <si>
     <t>concat node</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GCN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5layers</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8layers</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Node2vec not used</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Node2vec</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2layers</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3layers</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>layer 3</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -346,7 +386,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -382,6 +422,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -686,8 +729,8 @@
   <dimension ref="A1:L49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E35" sqref="E35"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1478,6 +1521,26 @@
         <v>23</v>
       </c>
     </row>
+    <row r="41" spans="1:11">
+      <c r="A41" s="3">
+        <v>0.90059999999999996</v>
+      </c>
+      <c r="B41" s="3">
+        <v>0.91010000000000002</v>
+      </c>
+      <c r="D41" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E41" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="F41" s="14">
+        <v>16</v>
+      </c>
+      <c r="G41" s="14" t="s">
+        <v>70</v>
+      </c>
+    </row>
     <row r="44" spans="1:11">
       <c r="A44" s="5">
         <v>41.587000000000003</v>
@@ -1488,10 +1551,10 @@
       <c r="C44" s="1">
         <v>0.01</v>
       </c>
-      <c r="D44" s="14" t="s">
+      <c r="D44" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E44" s="14"/>
+      <c r="E44" s="15"/>
       <c r="H44" s="1" t="s">
         <v>30</v>
       </c>
@@ -1515,10 +1578,10 @@
       <c r="C45" s="4">
         <v>0.01</v>
       </c>
-      <c r="D45" s="14" t="s">
+      <c r="D45" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E45" s="14"/>
+      <c r="E45" s="15"/>
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
       <c r="H45" s="4" t="s">
@@ -1544,10 +1607,10 @@
       <c r="C46" s="5">
         <v>0.01</v>
       </c>
-      <c r="D46" s="14" t="s">
+      <c r="D46" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E46" s="14"/>
+      <c r="E46" s="15"/>
       <c r="H46" s="1" t="s">
         <v>33</v>
       </c>
@@ -1571,10 +1634,10 @@
       <c r="C47" s="5">
         <v>0.01</v>
       </c>
-      <c r="D47" s="14" t="s">
+      <c r="D47" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E47" s="14"/>
+      <c r="E47" s="15"/>
       <c r="H47" s="1" t="s">
         <v>34</v>
       </c>
@@ -1598,10 +1661,10 @@
       <c r="C48" s="5">
         <v>0.01</v>
       </c>
-      <c r="D48" s="14" t="s">
+      <c r="D48" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E48" s="14"/>
+      <c r="E48" s="15"/>
       <c r="F48" s="5"/>
       <c r="G48" s="5"/>
       <c r="H48" s="5" t="s">
@@ -1623,10 +1686,10 @@
       <c r="C49" s="5">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="D49" s="14" t="s">
+      <c r="D49" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E49" s="14"/>
+      <c r="E49" s="15"/>
       <c r="F49" s="5"/>
       <c r="G49" s="5"/>
       <c r="H49" s="5" t="s">
@@ -1659,11 +1722,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{615B164C-2941-49E7-A89D-E66BEB08CEB9}">
-  <dimension ref="A1:M50"/>
+  <dimension ref="A1:M57"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E49" sqref="E49:M49"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G54" sqref="G54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2925,6 +2988,63 @@
         <v>60</v>
       </c>
     </row>
+    <row r="54" spans="1:13">
+      <c r="A54" s="5">
+        <v>60</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E54" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13">
+      <c r="A55" s="5">
+        <v>62.28</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C55" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="E55" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="F55" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13">
+      <c r="A56" s="5">
+        <v>62.85</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C56" s="13">
+        <v>0.01</v>
+      </c>
+      <c r="D56" s="13"/>
+      <c r="E56" s="13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13">
+      <c r="A57" s="5">
+        <v>69.58</v>
+      </c>
+      <c r="B57" s="5">
+        <v>72.959999999999994</v>
+      </c>
+      <c r="E57" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="F57" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2943,34 +3063,34 @@
   <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="3" spans="1:26">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
-      <c r="O3" s="14"/>
-      <c r="P3" s="14"/>
-      <c r="Q3" s="14"/>
-      <c r="R3" s="14"/>
-      <c r="S3" s="14"/>
-      <c r="T3" s="14"/>
-      <c r="U3" s="14"/>
-      <c r="V3" s="14"/>
-      <c r="W3" s="14"/>
-      <c r="X3" s="14"/>
-      <c r="Y3" s="14"/>
-      <c r="Z3" s="14"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="15"/>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="15"/>
+      <c r="R3" s="15"/>
+      <c r="S3" s="15"/>
+      <c r="T3" s="15"/>
+      <c r="U3" s="15"/>
+      <c r="V3" s="15"/>
+      <c r="W3" s="15"/>
+      <c r="X3" s="15"/>
+      <c r="Y3" s="15"/>
+      <c r="Z3" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>